<commit_message>
Phone Number Search Validation Add
</commit_message>
<xml_diff>
--- a/VarNameChanges.xlsx
+++ b/VarNameChanges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal Karan\Documents\GitHub\Intermediate-App-Dev-CQRS-OLTP-Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04225620-BA99-495A-82A8-C9A6A90D84F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1E85A9-EA66-4195-B1B4-42F02932BE2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13667" windowHeight="4913" xr2:uid="{338484CB-272E-451C-9394-80861DFE9DBE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Before:</t>
   </si>
@@ -47,20 +47,74 @@
     <t>newRental</t>
   </si>
   <si>
-    <t>btnCreateRental</t>
-  </si>
-  <si>
     <t>HIDDEN_LABEL_selectedCustomerID</t>
   </si>
   <si>
     <t>lblCstmrId</t>
+  </si>
+  <si>
+    <t>PhoneNumberInput</t>
+  </si>
+  <si>
+    <t>phoneNumberSubmitBtn</t>
+  </si>
+  <si>
+    <t>lblCstmrPN</t>
+  </si>
+  <si>
+    <t>btnCstmrSearch</t>
+  </si>
+  <si>
+    <t>selectedCustomerName</t>
+  </si>
+  <si>
+    <t>selectedCustomerAddress</t>
+  </si>
+  <si>
+    <t>selectedCustomerCity</t>
+  </si>
+  <si>
+    <t>lblName</t>
+  </si>
+  <si>
+    <t>lblAddress</t>
+  </si>
+  <si>
+    <t>lblCity</t>
+  </si>
+  <si>
+    <t>creditcardinput</t>
+  </si>
+  <si>
+    <t>lblCrdtCrd</t>
+  </si>
+  <si>
+    <t>btnNew</t>
+  </si>
+  <si>
+    <t>applyCoupon</t>
+  </si>
+  <si>
+    <t>couponinput</t>
+  </si>
+  <si>
+    <t>LinkButton4</t>
+  </si>
+  <si>
+    <t>btnCancel</t>
+  </si>
+  <si>
+    <t>lblCpnId</t>
+  </si>
+  <si>
+    <t>btnApplyCpn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,13 +122,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929D4D76-1734-4DA8-A207-F6E778BE7FAC}">
-  <dimension ref="B1:C4"/>
+  <dimension ref="B1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -426,30 +505,119 @@
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B3" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B4" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>